<commit_message>
minor fixes for basic from excel
</commit_message>
<xml_diff>
--- a/dist/assets/data/spider-persistent.xlsx
+++ b/dist/assets/data/spider-persistent.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11113"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/devlan/Repos/research/data-forensics/dist/assets/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88004D25-5702-3D4D-B017-6CFF19F1895B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26055" windowHeight="11115"/>
+    <workbookView xWindow="19200" yWindow="500" windowWidth="19200" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet5" sheetId="5" r:id="rId1"/>
@@ -99,7 +105,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -165,7 +171,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -440,30 +446,30 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J494"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J480"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A454" workbookViewId="0">
+      <selection activeCell="B489" sqref="B489"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" customWidth="1"/>
-    <col min="2" max="5" width="14.140625" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" customWidth="1"/>
+    <col min="2" max="5" width="14.1640625" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
     <col min="7" max="7" width="17" customWidth="1"/>
     <col min="8" max="10" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -495,7 +501,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -527,7 +533,7 @@
         <v>253.06</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -559,7 +565,7 @@
         <v>456.28</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -591,7 +597,7 @@
         <v>262.63</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -623,7 +629,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
@@ -655,7 +661,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
@@ -687,7 +693,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>2</v>
       </c>
@@ -719,7 +725,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
@@ -751,7 +757,7 @@
         <v>382.53</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
@@ -783,7 +789,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>2</v>
       </c>
@@ -815,7 +821,7 @@
         <v>517.13</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
@@ -847,7 +853,7 @@
         <v>512.30999999999995</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
@@ -879,7 +885,7 @@
         <v>300.61</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>2</v>
       </c>
@@ -911,7 +917,7 @@
         <v>512.34</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>2</v>
       </c>
@@ -943,7 +949,7 @@
         <v>512.34</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>2</v>
       </c>
@@ -975,7 +981,7 @@
         <v>217.97</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>2</v>
       </c>
@@ -1007,7 +1013,7 @@
         <v>136.13</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>2</v>
       </c>
@@ -1039,7 +1045,7 @@
         <v>54.62</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>2</v>
       </c>
@@ -1071,7 +1077,7 @@
         <v>517.75</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>2</v>
       </c>
@@ -1103,7 +1109,7 @@
         <v>409.63</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>2</v>
       </c>
@@ -1135,7 +1141,7 @@
         <v>276.10000000000002</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>2</v>
       </c>
@@ -1167,7 +1173,7 @@
         <v>186.9</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>2</v>
       </c>
@@ -1199,7 +1205,7 @@
         <v>62.69</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>2</v>
       </c>
@@ -1231,7 +1237,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>2</v>
       </c>
@@ -1263,7 +1269,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>2</v>
       </c>
@@ -1295,7 +1301,7 @@
         <v>12.22</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>2</v>
       </c>
@@ -1327,7 +1333,7 @@
         <v>155.21</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>2</v>
       </c>
@@ -1359,7 +1365,7 @@
         <v>524.32000000000005</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>2</v>
       </c>
@@ -1391,7 +1397,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>2</v>
       </c>
@@ -1423,7 +1429,7 @@
         <v>264.13</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>1</v>
       </c>
@@ -1455,7 +1461,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>1</v>
       </c>
@@ -1487,7 +1493,7 @@
         <v>148.03</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>1</v>
       </c>
@@ -1519,7 +1525,7 @@
         <v>75.599999999999994</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>1</v>
       </c>
@@ -1551,7 +1557,7 @@
         <v>502.06</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>1</v>
       </c>
@@ -1583,7 +1589,7 @@
         <v>32.94</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>1</v>
       </c>
@@ -1615,7 +1621,7 @@
         <v>493.87</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>1</v>
       </c>
@@ -1647,7 +1653,7 @@
         <v>157.49</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>1</v>
       </c>
@@ -1679,7 +1685,7 @@
         <v>500.2</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>1</v>
       </c>
@@ -1711,7 +1717,7 @@
         <v>321.87</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>1</v>
       </c>
@@ -1743,7 +1749,7 @@
         <v>506.47</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>1</v>
       </c>
@@ -1775,7 +1781,7 @@
         <v>131.28</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>1</v>
       </c>
@@ -1807,7 +1813,7 @@
         <v>502.31</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>1</v>
       </c>
@@ -1839,7 +1845,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>1</v>
       </c>
@@ -1871,7 +1877,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>1</v>
       </c>
@@ -1903,7 +1909,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>3</v>
       </c>
@@ -1935,7 +1941,7 @@
         <v>119.81</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>3</v>
       </c>
@@ -1967,7 +1973,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>3</v>
       </c>
@@ -1999,7 +2005,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>3</v>
       </c>
@@ -2031,7 +2037,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>11</v>
       </c>
@@ -2063,7 +2069,7 @@
         <v>489.22</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>11</v>
       </c>
@@ -2095,7 +2101,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>11</v>
       </c>
@@ -2127,7 +2133,7 @@
         <v>435.03</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>11</v>
       </c>
@@ -2159,7 +2165,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>11</v>
       </c>
@@ -2191,7 +2197,7 @@
         <v>288.47000000000003</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>11</v>
       </c>
@@ -2223,7 +2229,7 @@
         <v>292.87</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>11</v>
       </c>
@@ -2255,7 +2261,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>11</v>
       </c>
@@ -2287,7 +2293,7 @@
         <v>304.52</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>11</v>
       </c>
@@ -2319,7 +2325,7 @@
         <v>182.91</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>11</v>
       </c>
@@ -2351,7 +2357,7 @@
         <v>248.53</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>11</v>
       </c>
@@ -2383,7 +2389,7 @@
         <v>559.29</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>11</v>
       </c>
@@ -2415,7 +2421,7 @@
         <v>262.54000000000002</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>11</v>
       </c>
@@ -2447,7 +2453,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>11</v>
       </c>
@@ -2479,7 +2485,7 @@
         <v>288.19</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>11</v>
       </c>
@@ -2511,7 +2517,7 @@
         <v>286.58999999999997</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>11</v>
       </c>
@@ -2543,7 +2549,7 @@
         <v>381.75</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>11</v>
       </c>
@@ -2575,7 +2581,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>11</v>
       </c>
@@ -2607,7 +2613,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>11</v>
       </c>
@@ -2639,7 +2645,7 @@
         <v>365.56</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>11</v>
       </c>
@@ -2671,7 +2677,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>11</v>
       </c>
@@ -2703,7 +2709,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>11</v>
       </c>
@@ -2735,7 +2741,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>11</v>
       </c>
@@ -2767,7 +2773,7 @@
         <v>236.63</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>11</v>
       </c>
@@ -2799,7 +2805,7 @@
         <v>174.16</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>11</v>
       </c>
@@ -2831,7 +2837,7 @@
         <v>367.66</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>11</v>
       </c>
@@ -2863,7 +2869,7 @@
         <v>168.72</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>11</v>
       </c>
@@ -2895,7 +2901,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>11</v>
       </c>
@@ -2927,7 +2933,7 @@
         <v>323.52</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>11</v>
       </c>
@@ -2959,7 +2965,7 @@
         <v>143.22</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>11</v>
       </c>
@@ -2991,7 +2997,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>11</v>
       </c>
@@ -3023,7 +3029,7 @@
         <v>174.16</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>11</v>
       </c>
@@ -3055,7 +3061,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>11</v>
       </c>
@@ -3087,7 +3093,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>11</v>
       </c>
@@ -3119,7 +3125,7 @@
         <v>79.55</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>11</v>
       </c>
@@ -3151,7 +3157,7 @@
         <v>260.33999999999997</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>11</v>
       </c>
@@ -3183,7 +3189,7 @@
         <v>85.75</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>11</v>
       </c>
@@ -3215,7 +3221,7 @@
         <v>51.32</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>11</v>
       </c>
@@ -3247,7 +3253,7 @@
         <v>22.06</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>11</v>
       </c>
@@ -3279,7 +3285,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>11</v>
       </c>
@@ -3311,7 +3317,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>11</v>
       </c>
@@ -3343,7 +3349,7 @@
         <v>268.79000000000002</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>11</v>
       </c>
@@ -3375,7 +3381,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>11</v>
       </c>
@@ -3407,7 +3413,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>11</v>
       </c>
@@ -3439,7 +3445,7 @@
         <v>304.52</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>11</v>
       </c>
@@ -3471,7 +3477,7 @@
         <v>182.91</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>11</v>
       </c>
@@ -3503,7 +3509,7 @@
         <v>248.53</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>5</v>
       </c>
@@ -3535,7 +3541,7 @@
         <v>545.80999999999995</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>5</v>
       </c>
@@ -3567,7 +3573,7 @@
         <v>154.22999999999999</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>5</v>
       </c>
@@ -3599,7 +3605,7 @@
         <v>456.46</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>5</v>
       </c>
@@ -3631,7 +3637,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>5</v>
       </c>
@@ -3663,7 +3669,7 @@
         <v>10.94</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>5</v>
       </c>
@@ -3695,7 +3701,7 @@
         <v>59.89</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
         <v>5</v>
       </c>
@@ -3727,7 +3733,7 @@
         <v>122.81</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
         <v>5</v>
       </c>
@@ -3759,7 +3765,7 @@
         <v>264.97000000000003</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
         <v>5</v>
       </c>
@@ -3791,7 +3797,7 @@
         <v>21.78</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
         <v>5</v>
       </c>
@@ -3823,7 +3829,7 @@
         <v>15.82</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
         <v>5</v>
       </c>
@@ -3855,7 +3861,7 @@
         <v>507.44</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
         <v>5</v>
       </c>
@@ -3887,7 +3893,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
         <v>5</v>
       </c>
@@ -3919,7 +3925,7 @@
         <v>429.31</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
         <v>5</v>
       </c>
@@ -3951,7 +3957,7 @@
         <v>290.77999999999997</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
         <v>5</v>
       </c>
@@ -3983,7 +3989,7 @@
         <v>103.64</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
         <v>5</v>
       </c>
@@ -4015,7 +4021,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
         <v>5</v>
       </c>
@@ -4047,7 +4053,7 @@
         <v>230.31</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
         <v>5</v>
       </c>
@@ -4079,7 +4085,7 @@
         <v>154.99</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
         <v>5</v>
       </c>
@@ -4111,7 +4117,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
         <v>5</v>
       </c>
@@ -4143,7 +4149,7 @@
         <v>85.69</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
         <v>5</v>
       </c>
@@ -4175,7 +4181,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
         <v>5</v>
       </c>
@@ -4207,7 +4213,7 @@
         <v>174.99</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
         <v>5</v>
       </c>
@@ -4239,7 +4245,7 @@
         <v>29.56</v>
       </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
         <v>5</v>
       </c>
@@ -4271,7 +4277,7 @@
         <v>257.87</v>
       </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
         <v>5</v>
       </c>
@@ -4303,7 +4309,7 @@
         <v>405.32</v>
       </c>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
         <v>5</v>
       </c>
@@ -4335,7 +4341,7 @@
         <v>541.97</v>
       </c>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
         <v>5</v>
       </c>
@@ -4367,7 +4373,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
         <v>5</v>
       </c>
@@ -4399,7 +4405,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
         <v>5</v>
       </c>
@@ -4431,7 +4437,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
         <v>5</v>
       </c>
@@ -4463,7 +4469,7 @@
         <v>181.41</v>
       </c>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
         <v>5</v>
       </c>
@@ -4495,7 +4501,7 @@
         <v>544.87</v>
       </c>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
         <v>5</v>
       </c>
@@ -4527,7 +4533,7 @@
         <v>51.99</v>
       </c>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
         <v>5</v>
       </c>
@@ -4559,7 +4565,7 @@
         <v>300.62</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
         <v>5</v>
       </c>
@@ -4591,7 +4597,7 @@
         <v>160.5</v>
       </c>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
         <v>5</v>
       </c>
@@ -4623,7 +4629,7 @@
         <v>321.77999999999997</v>
       </c>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
         <v>5</v>
       </c>
@@ -4655,7 +4661,7 @@
         <v>484.75</v>
       </c>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
         <v>5</v>
       </c>
@@ -4687,7 +4693,7 @@
         <v>484.75</v>
       </c>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
         <v>5</v>
       </c>
@@ -4719,7 +4725,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
         <v>5</v>
       </c>
@@ -4751,7 +4757,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
         <v>5</v>
       </c>
@@ -4783,7 +4789,7 @@
         <v>11.85</v>
       </c>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
         <v>5</v>
       </c>
@@ -4815,7 +4821,7 @@
         <v>96.84</v>
       </c>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
         <v>5</v>
       </c>
@@ -4847,7 +4853,7 @@
         <v>18.190000000000001</v>
       </c>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
         <v>5</v>
       </c>
@@ -4879,7 +4885,7 @@
         <v>157.47</v>
       </c>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
         <v>5</v>
       </c>
@@ -4911,7 +4917,7 @@
         <v>246.84</v>
       </c>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
         <v>5</v>
       </c>
@@ -4943,7 +4949,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
         <v>5</v>
       </c>
@@ -4975,7 +4981,7 @@
         <v>69.19</v>
       </c>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
         <v>5</v>
       </c>
@@ -5007,7 +5013,7 @@
         <v>489.22</v>
       </c>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
         <v>5</v>
       </c>
@@ -5039,7 +5045,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
         <v>5</v>
       </c>
@@ -5071,7 +5077,7 @@
         <v>20.350000000000001</v>
       </c>
     </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
         <v>5</v>
       </c>
@@ -5103,7 +5109,7 @@
         <v>282.33999999999997</v>
       </c>
     </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
         <v>5</v>
       </c>
@@ -5135,7 +5141,7 @@
         <v>272.54000000000002</v>
       </c>
     </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
         <v>5</v>
       </c>
@@ -5167,7 +5173,7 @@
         <v>195.31</v>
       </c>
     </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
         <v>5</v>
       </c>
@@ -5199,7 +5205,7 @@
         <v>346.38</v>
       </c>
     </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
         <v>5</v>
       </c>
@@ -5231,7 +5237,7 @@
         <v>98.19</v>
       </c>
     </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
         <v>9</v>
       </c>
@@ -5263,7 +5269,7 @@
         <v>313.39999999999998</v>
       </c>
     </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
         <v>9</v>
       </c>
@@ -5295,7 +5301,7 @@
         <v>540.04</v>
       </c>
     </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
         <v>9</v>
       </c>
@@ -5327,7 +5333,7 @@
         <v>132.31</v>
       </c>
     </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
         <v>9</v>
       </c>
@@ -5359,7 +5365,7 @@
         <v>234.47</v>
       </c>
     </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
         <v>9</v>
       </c>
@@ -5391,7 +5397,7 @@
         <v>130.03</v>
       </c>
     </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
         <v>9</v>
       </c>
@@ -5423,7 +5429,7 @@
         <v>173.94</v>
       </c>
     </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
         <v>9</v>
       </c>
@@ -5455,7 +5461,7 @@
         <v>128.59</v>
       </c>
     </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
         <v>9</v>
       </c>
@@ -5487,7 +5493,7 @@
         <v>503.29</v>
       </c>
     </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
         <v>9</v>
       </c>
@@ -5519,7 +5525,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
         <v>9</v>
       </c>
@@ -5551,7 +5557,7 @@
         <v>424.84</v>
       </c>
     </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
         <v>9</v>
       </c>
@@ -5583,7 +5589,7 @@
         <v>192.68</v>
       </c>
     </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
         <v>9</v>
       </c>
@@ -5615,7 +5621,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
         <v>9</v>
       </c>
@@ -5647,7 +5653,7 @@
         <v>135.18</v>
       </c>
     </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
         <v>9</v>
       </c>
@@ -5679,7 +5685,7 @@
         <v>26.09</v>
       </c>
     </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
         <v>9</v>
       </c>
@@ -5711,7 +5717,7 @@
         <v>414.22</v>
       </c>
     </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
         <v>9</v>
       </c>
@@ -5743,7 +5749,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="s">
         <v>9</v>
       </c>
@@ -5775,7 +5781,7 @@
         <v>130.72</v>
       </c>
     </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A167" s="1" t="s">
         <v>9</v>
       </c>
@@ -5807,7 +5813,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A168" s="1" t="s">
         <v>9</v>
       </c>
@@ -5839,7 +5845,7 @@
         <v>180.71</v>
       </c>
     </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A169" s="1" t="s">
         <v>9</v>
       </c>
@@ -5871,7 +5877,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A170" s="1" t="s">
         <v>9</v>
       </c>
@@ -5903,7 +5909,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A171" s="1" t="s">
         <v>9</v>
       </c>
@@ -5935,7 +5941,7 @@
         <v>328.25</v>
       </c>
     </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A172" s="1" t="s">
         <v>9</v>
       </c>
@@ -5967,7 +5973,7 @@
         <v>321.77999999999997</v>
       </c>
     </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A173" s="1" t="s">
         <v>9</v>
       </c>
@@ -5999,7 +6005,7 @@
         <v>290.22000000000003</v>
       </c>
     </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A174" s="1" t="s">
         <v>9</v>
       </c>
@@ -6031,7 +6037,7 @@
         <v>327.82</v>
       </c>
     </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A175" s="1" t="s">
         <v>9</v>
       </c>
@@ -6063,7 +6069,7 @@
         <v>550.12</v>
       </c>
     </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
         <v>9</v>
       </c>
@@ -6095,7 +6101,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A177" s="1" t="s">
         <v>9</v>
       </c>
@@ -6127,7 +6133,7 @@
         <v>500.2</v>
       </c>
     </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A178" s="1" t="s">
         <v>9</v>
       </c>
@@ -6159,7 +6165,7 @@
         <v>177.94</v>
       </c>
     </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A179" s="1" t="s">
         <v>9</v>
       </c>
@@ -6191,7 +6197,7 @@
         <v>398.4</v>
       </c>
     </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A180" s="1" t="s">
         <v>9</v>
       </c>
@@ -6223,7 +6229,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A181" s="1" t="s">
         <v>9</v>
       </c>
@@ -6255,7 +6261,7 @@
         <v>235.25</v>
       </c>
     </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A182" s="1" t="s">
         <v>9</v>
       </c>
@@ -6287,7 +6293,7 @@
         <v>143.09</v>
       </c>
     </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A183" s="1" t="s">
         <v>9</v>
       </c>
@@ -6319,7 +6325,7 @@
         <v>370.03</v>
       </c>
     </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A184" s="1" t="s">
         <v>9</v>
       </c>
@@ -6351,7 +6357,7 @@
         <v>340.81</v>
       </c>
     </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A185" s="1" t="s">
         <v>9</v>
       </c>
@@ -6383,7 +6389,7 @@
         <v>232.56</v>
       </c>
     </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A186" s="1" t="s">
         <v>9</v>
       </c>
@@ -6415,7 +6421,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A187" s="1" t="s">
         <v>9</v>
       </c>
@@ -6447,7 +6453,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A188" s="1" t="s">
         <v>9</v>
       </c>
@@ -6479,7 +6485,7 @@
         <v>259.22000000000003</v>
       </c>
     </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A189" s="1" t="s">
         <v>9</v>
       </c>
@@ -6511,7 +6517,7 @@
         <v>86.82</v>
       </c>
     </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A190" s="1" t="s">
         <v>9</v>
       </c>
@@ -6543,7 +6549,7 @@
         <v>304.83999999999997</v>
       </c>
     </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A191" s="1" t="s">
         <v>9</v>
       </c>
@@ -6575,7 +6581,7 @@
         <v>172.22</v>
       </c>
     </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A192" s="1" t="s">
         <v>9</v>
       </c>
@@ -6607,7 +6613,7 @@
         <v>212.64</v>
       </c>
     </row>
-    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A193" s="1" t="s">
         <v>9</v>
       </c>
@@ -6639,7 +6645,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A194" s="1" t="s">
         <v>9</v>
       </c>
@@ -6671,7 +6677,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A195" s="1" t="s">
         <v>9</v>
       </c>
@@ -6703,7 +6709,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A196" s="1" t="s">
         <v>9</v>
       </c>
@@ -6735,7 +6741,7 @@
         <v>369.06</v>
       </c>
     </row>
-    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A197" s="1" t="s">
         <v>9</v>
       </c>
@@ -6767,7 +6773,7 @@
         <v>395.78</v>
       </c>
     </row>
-    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A198" s="1" t="s">
         <v>9</v>
       </c>
@@ -6799,7 +6805,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A199" s="1" t="s">
         <v>9</v>
       </c>
@@ -6831,7 +6837,7 @@
         <v>300.25</v>
       </c>
     </row>
-    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A200" s="1" t="s">
         <v>9</v>
       </c>
@@ -6863,7 +6869,7 @@
         <v>154.75</v>
       </c>
     </row>
-    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A201" s="1" t="s">
         <v>9</v>
       </c>
@@ -6895,7 +6901,7 @@
         <v>265.45</v>
       </c>
     </row>
-    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A202" s="1" t="s">
         <v>9</v>
       </c>
@@ -6927,7 +6933,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A203" s="1" t="s">
         <v>9</v>
       </c>
@@ -6959,7 +6965,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A204" s="1" t="s">
         <v>9</v>
       </c>
@@ -6991,7 +6997,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A205" s="1" t="s">
         <v>9</v>
       </c>
@@ -7023,7 +7029,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A206" s="1" t="s">
         <v>9</v>
       </c>
@@ -7055,7 +7061,7 @@
         <v>68.28</v>
       </c>
     </row>
-    <row r="207" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A207" s="1" t="s">
         <v>9</v>
       </c>
@@ -7087,7 +7093,7 @@
         <v>135.91</v>
       </c>
     </row>
-    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A208" s="1" t="s">
         <v>9</v>
       </c>
@@ -7119,7 +7125,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="209" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A209" s="1" t="s">
         <v>9</v>
       </c>
@@ -7151,7 +7157,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="210" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A210" s="1" t="s">
         <v>9</v>
       </c>
@@ -7183,7 +7189,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A211" s="1" t="s">
         <v>9</v>
       </c>
@@ -7215,7 +7221,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A212" s="1" t="s">
         <v>9</v>
       </c>
@@ -7247,7 +7253,7 @@
         <v>211.58</v>
       </c>
     </row>
-    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A213" s="1" t="s">
         <v>9</v>
       </c>
@@ -7279,7 +7285,7 @@
         <v>355.4</v>
       </c>
     </row>
-    <row r="214" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A214" s="1" t="s">
         <v>9</v>
       </c>
@@ -7311,7 +7317,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A215" s="1" t="s">
         <v>9</v>
       </c>
@@ -7343,7 +7349,7 @@
         <v>462.45</v>
       </c>
     </row>
-    <row r="216" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A216" s="1" t="s">
         <v>9</v>
       </c>
@@ -7375,7 +7381,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="217" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A217" s="1" t="s">
         <v>9</v>
       </c>
@@ -7407,7 +7413,7 @@
         <v>482.53</v>
       </c>
     </row>
-    <row r="218" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A218" s="8" t="s">
         <v>12</v>
       </c>
@@ -7439,7 +7445,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="219" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A219" s="1" t="s">
         <v>12</v>
       </c>
@@ -7471,7 +7477,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="220" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A220" s="1" t="s">
         <v>12</v>
       </c>
@@ -7503,7 +7509,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="221" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A221" s="8" t="s">
         <v>12</v>
       </c>
@@ -7535,7 +7541,7 @@
         <v>448.5</v>
       </c>
     </row>
-    <row r="222" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A222" s="1" t="s">
         <v>12</v>
       </c>
@@ -7567,7 +7573,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="223" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A223" s="8" t="s">
         <v>12</v>
       </c>
@@ -7599,7 +7605,7 @@
         <v>341.12</v>
       </c>
     </row>
-    <row r="224" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A224" s="8" t="s">
         <v>12</v>
       </c>
@@ -7631,7 +7637,7 @@
         <v>521.42999999999995</v>
       </c>
     </row>
-    <row r="225" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A225" s="1" t="s">
         <v>12</v>
       </c>
@@ -7663,7 +7669,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="226" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A226" s="8" t="s">
         <v>12</v>
       </c>
@@ -7695,7 +7701,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="227" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A227" s="1" t="s">
         <v>12</v>
       </c>
@@ -7727,7 +7733,7 @@
         <v>407.97</v>
       </c>
     </row>
-    <row r="228" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A228" s="8" t="s">
         <v>12</v>
       </c>
@@ -7759,7 +7765,7 @@
         <v>286.58999999999997</v>
       </c>
     </row>
-    <row r="229" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A229" s="1" t="s">
         <v>12</v>
       </c>
@@ -7791,7 +7797,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="230" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A230" s="8" t="s">
         <v>12</v>
       </c>
@@ -7823,7 +7829,7 @@
         <v>294.93</v>
       </c>
     </row>
-    <row r="231" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A231" s="1" t="s">
         <v>12</v>
       </c>
@@ -7855,7 +7861,7 @@
         <v>14.72</v>
       </c>
     </row>
-    <row r="232" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A232" s="1" t="s">
         <v>12</v>
       </c>
@@ -7887,7 +7893,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="233" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A233" s="8" t="s">
         <v>12</v>
       </c>
@@ -7919,7 +7925,7 @@
         <v>566.32000000000005</v>
       </c>
     </row>
-    <row r="234" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A234" s="1" t="s">
         <v>12</v>
       </c>
@@ -7951,7 +7957,7 @@
         <v>152.28</v>
       </c>
     </row>
-    <row r="235" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A235" s="8" t="s">
         <v>12</v>
       </c>
@@ -7983,7 +7989,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="236" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A236" s="8" t="s">
         <v>12</v>
       </c>
@@ -8015,7 +8021,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="237" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A237" s="1" t="s">
         <v>12</v>
       </c>
@@ -8047,7 +8053,7 @@
         <v>454.61</v>
       </c>
     </row>
-    <row r="238" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A238" s="8" t="s">
         <v>12</v>
       </c>
@@ -8079,7 +8085,7 @@
         <v>129.47</v>
       </c>
     </row>
-    <row r="239" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A239" s="1" t="s">
         <v>12</v>
       </c>
@@ -8111,7 +8117,7 @@
         <v>155.66</v>
       </c>
     </row>
-    <row r="240" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A240" s="8" t="s">
         <v>12</v>
       </c>
@@ -8143,7 +8149,7 @@
         <v>578.88</v>
       </c>
     </row>
-    <row r="241" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A241" s="1" t="s">
         <v>12</v>
       </c>
@@ -8175,7 +8181,7 @@
         <v>512.34</v>
       </c>
     </row>
-    <row r="242" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A242" s="8" t="s">
         <v>12</v>
       </c>
@@ -8207,7 +8213,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="243" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A243" s="1" t="s">
         <v>12</v>
       </c>
@@ -8239,7 +8245,7 @@
         <v>48.92</v>
       </c>
     </row>
-    <row r="244" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A244" s="1" t="s">
         <v>12</v>
       </c>
@@ -8271,7 +8277,7 @@
         <v>522.30999999999995</v>
       </c>
     </row>
-    <row r="245" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A245" s="8" t="s">
         <v>12</v>
       </c>
@@ -8303,7 +8309,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="246" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A246" s="1" t="s">
         <v>12</v>
       </c>
@@ -8335,7 +8341,7 @@
         <v>172.13</v>
       </c>
     </row>
-    <row r="247" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A247" s="8" t="s">
         <v>12</v>
       </c>
@@ -8367,7 +8373,7 @@
         <v>479.12</v>
       </c>
     </row>
-    <row r="248" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A248" s="1" t="s">
         <v>12</v>
       </c>
@@ -8399,7 +8405,7 @@
         <v>123.54</v>
       </c>
     </row>
-    <row r="249" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A249" s="8" t="s">
         <v>12</v>
       </c>
@@ -8431,7 +8437,7 @@
         <v>96.94</v>
       </c>
     </row>
-    <row r="250" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A250" s="1" t="s">
         <v>12</v>
       </c>
@@ -8463,7 +8469,7 @@
         <v>47.97</v>
       </c>
     </row>
-    <row r="251" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A251" s="8" t="s">
         <v>12</v>
       </c>
@@ -8495,7 +8501,7 @@
         <v>186.59</v>
       </c>
     </row>
-    <row r="252" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A252" s="1" t="s">
         <v>12</v>
       </c>
@@ -8527,7 +8533,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="253" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A253" s="8" t="s">
         <v>12</v>
       </c>
@@ -8559,7 +8565,7 @@
         <v>517.75</v>
       </c>
     </row>
-    <row r="254" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A254" s="8" t="s">
         <v>12</v>
       </c>
@@ -8591,7 +8597,7 @@
         <v>36.590000000000003</v>
       </c>
     </row>
-    <row r="255" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A255" s="1" t="s">
         <v>12</v>
       </c>
@@ -8623,7 +8629,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="256" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A256" s="8" t="s">
         <v>12</v>
       </c>
@@ -8655,7 +8661,7 @@
         <v>490.37</v>
       </c>
     </row>
-    <row r="257" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A257" s="1" t="s">
         <v>12</v>
       </c>
@@ -8687,7 +8693,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="258" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A258" s="8" t="s">
         <v>12</v>
       </c>
@@ -8719,7 +8725,7 @@
         <v>564.20000000000005</v>
       </c>
     </row>
-    <row r="259" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A259" s="1" t="s">
         <v>12</v>
       </c>
@@ -8751,7 +8757,7 @@
         <v>564.75</v>
       </c>
     </row>
-    <row r="260" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A260" s="8" t="s">
         <v>12</v>
       </c>
@@ -8783,7 +8789,7 @@
         <v>177.87</v>
       </c>
     </row>
-    <row r="261" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A261" s="1" t="s">
         <v>12</v>
       </c>
@@ -8815,7 +8821,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="262" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A262" s="8" t="s">
         <v>12</v>
       </c>
@@ -8847,7 +8853,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="263" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A263" s="8" t="s">
         <v>12</v>
       </c>
@@ -8879,7 +8885,7 @@
         <v>517.75</v>
       </c>
     </row>
-    <row r="264" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A264" s="1" t="s">
         <v>12</v>
       </c>
@@ -8911,7 +8917,7 @@
         <v>589.94000000000005</v>
       </c>
     </row>
-    <row r="265" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A265" s="8" t="s">
         <v>12</v>
       </c>
@@ -8943,7 +8949,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="266" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A266" s="1" t="s">
         <v>12</v>
       </c>
@@ -8975,7 +8981,7 @@
         <v>64.13</v>
       </c>
     </row>
-    <row r="267" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A267" s="8" t="s">
         <v>12</v>
       </c>
@@ -9007,7 +9013,7 @@
         <v>580.84</v>
       </c>
     </row>
-    <row r="268" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A268" s="1" t="s">
         <v>12</v>
       </c>
@@ -9039,7 +9045,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="269" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A269" s="1" t="s">
         <v>12</v>
       </c>
@@ -9071,7 +9077,7 @@
         <v>359.62</v>
       </c>
     </row>
-    <row r="270" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A270" s="8" t="s">
         <v>12</v>
       </c>
@@ -9103,7 +9109,7 @@
         <v>124.91</v>
       </c>
     </row>
-    <row r="271" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A271" s="1" t="s">
         <v>12</v>
       </c>
@@ -9135,7 +9141,7 @@
         <v>578.71</v>
       </c>
     </row>
-    <row r="272" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A272" s="8" t="s">
         <v>12</v>
       </c>
@@ -9167,7 +9173,7 @@
         <v>291.31</v>
       </c>
     </row>
-    <row r="273" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A273" s="1" t="s">
         <v>12</v>
       </c>
@@ -9199,7 +9205,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="274" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A274" s="1" t="s">
         <v>12</v>
       </c>
@@ -9231,7 +9237,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="275" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A275" s="8" t="s">
         <v>12</v>
       </c>
@@ -9263,7 +9269,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="276" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A276" s="1" t="s">
         <v>12</v>
       </c>
@@ -9295,7 +9301,7 @@
         <v>74.790000000000006</v>
       </c>
     </row>
-    <row r="277" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A277" s="8" t="s">
         <v>12</v>
       </c>
@@ -9327,7 +9333,7 @@
         <v>415.47</v>
       </c>
     </row>
-    <row r="278" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A278" s="1" t="s">
         <v>12</v>
       </c>
@@ -9359,7 +9365,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="279" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A279" s="8" t="s">
         <v>12</v>
       </c>
@@ -9391,7 +9397,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="280" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A280" s="8" t="s">
         <v>12</v>
       </c>
@@ -9423,7 +9429,7 @@
         <v>265.45</v>
       </c>
     </row>
-    <row r="281" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A281" s="1" t="s">
         <v>12</v>
       </c>
@@ -9455,7 +9461,7 @@
         <v>184.56</v>
       </c>
     </row>
-    <row r="282" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A282" s="1" t="s">
         <v>12</v>
       </c>
@@ -9487,7 +9493,7 @@
         <v>208.78</v>
       </c>
     </row>
-    <row r="283" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A283" s="8" t="s">
         <v>12</v>
       </c>
@@ -9519,7 +9525,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="284" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A284" s="8" t="s">
         <v>12</v>
       </c>
@@ -9551,7 +9557,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="285" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A285" s="1" t="s">
         <v>12</v>
       </c>
@@ -9583,7 +9589,7 @@
         <v>589.94000000000005</v>
       </c>
     </row>
-    <row r="286" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A286" s="8" t="s">
         <v>12</v>
       </c>
@@ -9615,7 +9621,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="287" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A287" s="1" t="s">
         <v>12</v>
       </c>
@@ -9647,7 +9653,7 @@
         <v>392.47</v>
       </c>
     </row>
-    <row r="288" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A288" s="8" t="s">
         <v>12</v>
       </c>
@@ -9679,7 +9685,7 @@
         <v>60.48</v>
       </c>
     </row>
-    <row r="289" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A289" s="8" t="s">
         <v>13</v>
       </c>
@@ -9711,7 +9717,7 @@
         <v>402.25</v>
       </c>
     </row>
-    <row r="290" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A290" s="1" t="s">
         <v>13</v>
       </c>
@@ -9743,7 +9749,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="291" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A291" s="1" t="s">
         <v>13</v>
       </c>
@@ -9775,7 +9781,7 @@
         <v>404.03</v>
       </c>
     </row>
-    <row r="292" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A292" s="1" t="s">
         <v>13</v>
       </c>
@@ -9807,7 +9813,7 @@
         <v>397.59</v>
       </c>
     </row>
-    <row r="293" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A293" s="1" t="s">
         <v>13</v>
       </c>
@@ -9839,7 +9845,7 @@
         <v>210.97</v>
       </c>
     </row>
-    <row r="294" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A294" s="8" t="s">
         <v>13</v>
       </c>
@@ -9871,7 +9877,7 @@
         <v>283.27999999999997</v>
       </c>
     </row>
-    <row r="295" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A295" s="1" t="s">
         <v>13</v>
       </c>
@@ -9903,7 +9909,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="296" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A296" s="8" t="s">
         <v>13</v>
       </c>
@@ -9935,7 +9941,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="297" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A297" s="8" t="s">
         <v>13</v>
       </c>
@@ -9967,7 +9973,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="298" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A298" s="1" t="s">
         <v>10</v>
       </c>
@@ -9999,7 +10005,7 @@
         <v>222.91</v>
       </c>
     </row>
-    <row r="299" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A299" s="1" t="s">
         <v>10</v>
       </c>
@@ -10031,7 +10037,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="300" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A300" s="1" t="s">
         <v>10</v>
       </c>
@@ -10063,7 +10069,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="301" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A301" s="1" t="s">
         <v>10</v>
       </c>
@@ -10095,7 +10101,7 @@
         <v>258.2</v>
       </c>
     </row>
-    <row r="302" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A302" s="1" t="s">
         <v>10</v>
       </c>
@@ -10127,7 +10133,7 @@
         <v>393.81</v>
       </c>
     </row>
-    <row r="303" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A303" s="1" t="s">
         <v>10</v>
       </c>
@@ -10159,7 +10165,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="304" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A304" s="1" t="s">
         <v>10</v>
       </c>
@@ -10191,7 +10197,7 @@
         <v>168.68</v>
       </c>
     </row>
-    <row r="305" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A305" s="1" t="s">
         <v>10</v>
       </c>
@@ -10223,7 +10229,7 @@
         <v>248.5</v>
       </c>
     </row>
-    <row r="306" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A306" s="1" t="s">
         <v>10</v>
       </c>
@@ -10255,7 +10261,7 @@
         <v>96.5</v>
       </c>
     </row>
-    <row r="307" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A307" s="1" t="s">
         <v>10</v>
       </c>
@@ -10287,7 +10293,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="308" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A308" s="1" t="s">
         <v>10</v>
       </c>
@@ -10319,7 +10325,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="309" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A309" s="1" t="s">
         <v>10</v>
       </c>
@@ -10351,7 +10357,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="310" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A310" s="1" t="s">
         <v>10</v>
       </c>
@@ -10383,7 +10389,7 @@
         <v>37.25</v>
       </c>
     </row>
-    <row r="311" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A311" s="1" t="s">
         <v>10</v>
       </c>
@@ -10415,7 +10421,7 @@
         <v>55.67</v>
       </c>
     </row>
-    <row r="312" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A312" s="1" t="s">
         <v>10</v>
       </c>
@@ -10447,7 +10453,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="313" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A313" s="1" t="s">
         <v>10</v>
       </c>
@@ -10479,7 +10485,7 @@
         <v>364.51</v>
       </c>
     </row>
-    <row r="314" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A314" s="1" t="s">
         <v>10</v>
       </c>
@@ -10511,7 +10517,7 @@
         <v>86.9</v>
       </c>
     </row>
-    <row r="315" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A315" s="1" t="s">
         <v>10</v>
       </c>
@@ -10543,7 +10549,7 @@
         <v>599.78</v>
       </c>
     </row>
-    <row r="316" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A316" s="1" t="s">
         <v>10</v>
       </c>
@@ -10575,7 +10581,7 @@
         <v>255.64</v>
       </c>
     </row>
-    <row r="317" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A317" s="1" t="s">
         <v>10</v>
       </c>
@@ -10607,7 +10613,7 @@
         <v>443.47</v>
       </c>
     </row>
-    <row r="318" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A318" s="1" t="s">
         <v>10</v>
       </c>
@@ -10639,7 +10645,7 @@
         <v>382.62</v>
       </c>
     </row>
-    <row r="319" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A319" s="1" t="s">
         <v>10</v>
       </c>
@@ -10671,7 +10677,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="320" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A320" s="1" t="s">
         <v>10</v>
       </c>
@@ -10703,7 +10709,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="321" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A321" s="1" t="s">
         <v>4</v>
       </c>
@@ -10735,7 +10741,7 @@
         <v>484.62</v>
       </c>
     </row>
-    <row r="322" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A322" s="1" t="s">
         <v>6</v>
       </c>
@@ -10767,7 +10773,7 @@
         <v>266.51</v>
       </c>
     </row>
-    <row r="323" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A323" s="1" t="s">
         <v>6</v>
       </c>
@@ -10799,7 +10805,7 @@
         <v>312.5</v>
       </c>
     </row>
-    <row r="324" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A324" s="1" t="s">
         <v>6</v>
       </c>
@@ -10831,7 +10837,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="325" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A325" s="1" t="s">
         <v>6</v>
       </c>
@@ -10863,7 +10869,7 @@
         <v>76.94</v>
       </c>
     </row>
-    <row r="326" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A326" s="1" t="s">
         <v>6</v>
       </c>
@@ -10895,7 +10901,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="327" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A327" s="1" t="s">
         <v>6</v>
       </c>
@@ -10927,7 +10933,7 @@
         <v>370.22</v>
       </c>
     </row>
-    <row r="328" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A328" s="1" t="s">
         <v>6</v>
       </c>
@@ -10959,7 +10965,7 @@
         <v>327.19</v>
       </c>
     </row>
-    <row r="329" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A329" s="1" t="s">
         <v>6</v>
       </c>
@@ -10991,7 +10997,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="330" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A330" s="1" t="s">
         <v>6</v>
       </c>
@@ -11023,7 +11029,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="331" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A331" s="1" t="s">
         <v>6</v>
       </c>
@@ -11055,7 +11061,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="332" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A332" s="1" t="s">
         <v>6</v>
       </c>
@@ -11087,7 +11093,7 @@
         <v>458.1</v>
       </c>
     </row>
-    <row r="333" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A333" s="1" t="s">
         <v>6</v>
       </c>
@@ -11119,7 +11125,7 @@
         <v>154.12</v>
       </c>
     </row>
-    <row r="334" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A334" s="1" t="s">
         <v>6</v>
       </c>
@@ -11151,7 +11157,7 @@
         <v>477.61</v>
       </c>
     </row>
-    <row r="335" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A335" s="1" t="s">
         <v>6</v>
       </c>
@@ -11183,7 +11189,7 @@
         <v>101.54</v>
       </c>
     </row>
-    <row r="336" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A336" s="1" t="s">
         <v>6</v>
       </c>
@@ -11215,7 +11221,7 @@
         <v>300.45</v>
       </c>
     </row>
-    <row r="337" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A337" s="1" t="s">
         <v>6</v>
       </c>
@@ -11247,7 +11253,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="338" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A338" s="1" t="s">
         <v>6</v>
       </c>
@@ -11279,7 +11285,7 @@
         <v>142.59</v>
       </c>
     </row>
-    <row r="339" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A339" s="1" t="s">
         <v>6</v>
       </c>
@@ -11311,7 +11317,7 @@
         <v>464.6</v>
       </c>
     </row>
-    <row r="340" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A340" s="1" t="s">
         <v>6</v>
       </c>
@@ -11343,7 +11349,7 @@
         <v>189.52</v>
       </c>
     </row>
-    <row r="341" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A341" s="1" t="s">
         <v>6</v>
       </c>
@@ -11375,7 +11381,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="342" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A342" s="1" t="s">
         <v>6</v>
       </c>
@@ -11407,7 +11413,7 @@
         <v>394.65</v>
       </c>
     </row>
-    <row r="343" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A343" s="1" t="s">
         <v>6</v>
       </c>
@@ -11439,7 +11445,7 @@
         <v>32.369999999999997</v>
       </c>
     </row>
-    <row r="344" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A344" s="1" t="s">
         <v>6</v>
       </c>
@@ -11471,7 +11477,7 @@
         <v>159.53</v>
       </c>
     </row>
-    <row r="345" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A345" s="1" t="s">
         <v>6</v>
       </c>
@@ -11503,7 +11509,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="346" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A346" s="1" t="s">
         <v>6</v>
       </c>
@@ -11535,7 +11541,7 @@
         <v>303.79000000000002</v>
       </c>
     </row>
-    <row r="347" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A347" s="1" t="s">
         <v>6</v>
       </c>
@@ -11567,7 +11573,7 @@
         <v>436.41</v>
       </c>
     </row>
-    <row r="348" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A348" s="1" t="s">
         <v>6</v>
       </c>
@@ -11599,7 +11605,7 @@
         <v>465.48</v>
       </c>
     </row>
-    <row r="349" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A349" s="1" t="s">
         <v>6</v>
       </c>
@@ -11631,7 +11637,7 @@
         <v>354.62</v>
       </c>
     </row>
-    <row r="350" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A350" s="1" t="s">
         <v>6</v>
       </c>
@@ -11663,7 +11669,7 @@
         <v>377.65</v>
       </c>
     </row>
-    <row r="351" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A351" s="1" t="s">
         <v>6</v>
       </c>
@@ -11695,7 +11701,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="352" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A352" s="1" t="s">
         <v>6</v>
       </c>
@@ -11727,7 +11733,7 @@
         <v>105.63</v>
       </c>
     </row>
-    <row r="353" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A353" s="1" t="s">
         <v>6</v>
       </c>
@@ -11759,7 +11765,7 @@
         <v>304.97000000000003</v>
       </c>
     </row>
-    <row r="354" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A354" s="1" t="s">
         <v>6</v>
       </c>
@@ -11791,7 +11797,7 @@
         <v>23.07</v>
       </c>
     </row>
-    <row r="355" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A355" s="1" t="s">
         <v>6</v>
       </c>
@@ -11823,7 +11829,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="356" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A356" s="1" t="s">
         <v>6</v>
       </c>
@@ -11855,7 +11861,7 @@
         <v>202.04</v>
       </c>
     </row>
-    <row r="357" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A357" s="1" t="s">
         <v>6</v>
       </c>
@@ -11887,7 +11893,7 @@
         <v>66.09</v>
       </c>
     </row>
-    <row r="358" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A358" s="1" t="s">
         <v>6</v>
       </c>
@@ -11919,7 +11925,7 @@
         <v>465.78</v>
       </c>
     </row>
-    <row r="359" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A359" s="1" t="s">
         <v>6</v>
       </c>
@@ -11951,7 +11957,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="360" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A360" s="1" t="s">
         <v>6</v>
       </c>
@@ -11983,7 +11989,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="361" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A361" s="1" t="s">
         <v>6</v>
       </c>
@@ -12015,7 +12021,7 @@
         <v>420.87</v>
       </c>
     </row>
-    <row r="362" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A362" s="1" t="s">
         <v>6</v>
       </c>
@@ -12047,7 +12053,7 @@
         <v>299.66000000000003</v>
       </c>
     </row>
-    <row r="363" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A363" s="1" t="s">
         <v>6</v>
       </c>
@@ -12079,7 +12085,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="364" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A364" s="1" t="s">
         <v>6</v>
       </c>
@@ -12111,7 +12117,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="365" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A365" s="1" t="s">
         <v>6</v>
       </c>
@@ -12143,7 +12149,7 @@
         <v>138.65</v>
       </c>
     </row>
-    <row r="366" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A366" s="1" t="s">
         <v>6</v>
       </c>
@@ -12175,7 +12181,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="367" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A367" s="1" t="s">
         <v>6</v>
       </c>
@@ -12207,7 +12213,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="368" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A368" s="1" t="s">
         <v>6</v>
       </c>
@@ -12239,7 +12245,7 @@
         <v>326.54000000000002</v>
       </c>
     </row>
-    <row r="369" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A369" s="1" t="s">
         <v>6</v>
       </c>
@@ -12271,7 +12277,7 @@
         <v>40.340000000000003</v>
       </c>
     </row>
-    <row r="370" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A370" s="1" t="s">
         <v>6</v>
       </c>
@@ -12303,7 +12309,7 @@
         <v>143.22</v>
       </c>
     </row>
-    <row r="371" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A371" s="1" t="s">
         <v>6</v>
       </c>
@@ -12335,7 +12341,7 @@
         <v>119.96</v>
       </c>
     </row>
-    <row r="372" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A372" s="1" t="s">
         <v>6</v>
       </c>
@@ -12367,7 +12373,7 @@
         <v>145.19</v>
       </c>
     </row>
-    <row r="373" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A373" s="1" t="s">
         <v>6</v>
       </c>
@@ -12399,7 +12405,7 @@
         <v>311.81</v>
       </c>
     </row>
-    <row r="374" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A374" s="1" t="s">
         <v>6</v>
       </c>
@@ -12431,7 +12437,7 @@
         <v>475.62</v>
       </c>
     </row>
-    <row r="375" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A375" s="1" t="s">
         <v>6</v>
       </c>
@@ -12463,7 +12469,7 @@
         <v>69.41</v>
       </c>
     </row>
-    <row r="376" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A376" s="1" t="s">
         <v>6</v>
       </c>
@@ -12495,7 +12501,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="377" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A377" s="1" t="s">
         <v>6</v>
       </c>
@@ -12527,7 +12533,7 @@
         <v>365.9</v>
       </c>
     </row>
-    <row r="378" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A378" s="1" t="s">
         <v>6</v>
       </c>
@@ -12559,7 +12565,7 @@
         <v>452.55</v>
       </c>
     </row>
-    <row r="379" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A379" s="1" t="s">
         <v>6</v>
       </c>
@@ -12591,7 +12597,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="380" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A380" s="1" t="s">
         <v>6</v>
       </c>
@@ -12623,7 +12629,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="381" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A381" s="1" t="s">
         <v>6</v>
       </c>
@@ -12655,7 +12661,7 @@
         <v>321.87</v>
       </c>
     </row>
-    <row r="382" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A382" s="1" t="s">
         <v>6</v>
       </c>
@@ -12687,7 +12693,7 @@
         <v>471.84</v>
       </c>
     </row>
-    <row r="383" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A383" s="1" t="s">
         <v>6</v>
       </c>
@@ -12719,7 +12725,7 @@
         <v>62.22</v>
       </c>
     </row>
-    <row r="384" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A384" s="1" t="s">
         <v>6</v>
       </c>
@@ -12751,7 +12757,7 @@
         <v>161.84</v>
       </c>
     </row>
-    <row r="385" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A385" s="1" t="s">
         <v>6</v>
       </c>
@@ -12783,7 +12789,7 @@
         <v>58.81</v>
       </c>
     </row>
-    <row r="386" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A386" s="1" t="s">
         <v>6</v>
       </c>
@@ -12815,7 +12821,7 @@
         <v>163.38999999999999</v>
       </c>
     </row>
-    <row r="387" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A387" s="1" t="s">
         <v>6</v>
       </c>
@@ -12847,7 +12853,7 @@
         <v>209.65</v>
       </c>
     </row>
-    <row r="388" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A388" s="1" t="s">
         <v>6</v>
       </c>
@@ -12879,7 +12885,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="389" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A389" s="1" t="s">
         <v>6</v>
       </c>
@@ -12911,7 +12917,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="390" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A390" s="1" t="s">
         <v>6</v>
       </c>
@@ -12943,7 +12949,7 @@
         <v>39.5</v>
       </c>
     </row>
-    <row r="391" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A391" s="1" t="s">
         <v>6</v>
       </c>
@@ -12975,7 +12981,7 @@
         <v>104.76</v>
       </c>
     </row>
-    <row r="392" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A392" s="1" t="s">
         <v>6</v>
       </c>
@@ -13007,7 +13013,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="393" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A393" s="1" t="s">
         <v>6</v>
       </c>
@@ -13039,7 +13045,7 @@
         <v>238.01</v>
       </c>
     </row>
-    <row r="394" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A394" s="1" t="s">
         <v>6</v>
       </c>
@@ -13071,7 +13077,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="395" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A395" s="1" t="s">
         <v>6</v>
       </c>
@@ -13103,7 +13109,7 @@
         <v>70.97</v>
       </c>
     </row>
-    <row r="396" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A396" s="1" t="s">
         <v>6</v>
       </c>
@@ -13135,7 +13141,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="397" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A397" s="1" t="s">
         <v>6</v>
       </c>
@@ -13167,7 +13173,7 @@
         <v>143.94</v>
       </c>
     </row>
-    <row r="398" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A398" s="1" t="s">
         <v>6</v>
       </c>
@@ -13199,7 +13205,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="399" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A399" s="1" t="s">
         <v>6</v>
       </c>
@@ -13231,7 +13237,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="400" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A400" s="1" t="s">
         <v>6</v>
       </c>
@@ -13263,7 +13269,7 @@
         <v>170.57</v>
       </c>
     </row>
-    <row r="401" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A401" s="1" t="s">
         <v>6</v>
       </c>
@@ -13295,7 +13301,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="402" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A402" s="1" t="s">
         <v>6</v>
       </c>
@@ -13327,7 +13333,7 @@
         <v>405.34</v>
       </c>
     </row>
-    <row r="403" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A403" s="1" t="s">
         <v>6</v>
       </c>
@@ -13359,7 +13365,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="404" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A404" s="1" t="s">
         <v>6</v>
       </c>
@@ -13391,7 +13397,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="405" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A405" s="1" t="s">
         <v>6</v>
       </c>
@@ -13423,7 +13429,7 @@
         <v>406.66</v>
       </c>
     </row>
-    <row r="406" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A406" s="1" t="s">
         <v>6</v>
       </c>
@@ -13455,7 +13461,7 @@
         <v>114.03</v>
       </c>
     </row>
-    <row r="407" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A407" s="1" t="s">
         <v>6</v>
       </c>
@@ -13487,7 +13493,7 @@
         <v>449.29</v>
       </c>
     </row>
-    <row r="408" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A408" s="1" t="s">
         <v>6</v>
       </c>
@@ -13519,7 +13525,7 @@
         <v>274.69</v>
       </c>
     </row>
-    <row r="409" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A409" s="1" t="s">
         <v>6</v>
       </c>
@@ -13551,7 +13557,7 @@
         <v>154.28</v>
       </c>
     </row>
-    <row r="410" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A410" s="1" t="s">
         <v>6</v>
       </c>
@@ -13583,7 +13589,7 @@
         <v>465.48</v>
       </c>
     </row>
-    <row r="411" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A411" s="1" t="s">
         <v>6</v>
       </c>
@@ -13615,7 +13621,7 @@
         <v>277.13</v>
       </c>
     </row>
-    <row r="412" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A412" s="1" t="s">
         <v>6</v>
       </c>
@@ -13647,7 +13653,7 @@
         <v>253.19</v>
       </c>
     </row>
-    <row r="413" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A413" s="1" t="s">
         <v>6</v>
       </c>
@@ -13679,7 +13685,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="414" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A414" s="1" t="s">
         <v>6</v>
       </c>
@@ -13711,7 +13717,7 @@
         <v>201.9</v>
       </c>
     </row>
-    <row r="415" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A415" s="1" t="s">
         <v>6</v>
       </c>
@@ -13743,7 +13749,7 @@
         <v>293.82</v>
       </c>
     </row>
-    <row r="416" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A416" s="1" t="s">
         <v>7</v>
       </c>
@@ -13775,7 +13781,7 @@
         <v>579.28</v>
       </c>
     </row>
-    <row r="417" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A417" s="1" t="s">
         <v>7</v>
       </c>
@@ -13807,7 +13813,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="418" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A418" s="1" t="s">
         <v>7</v>
       </c>
@@ -13839,7 +13845,7 @@
         <v>144.47</v>
       </c>
     </row>
-    <row r="419" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A419" s="1" t="s">
         <v>7</v>
       </c>
@@ -13871,7 +13877,7 @@
         <v>138.97</v>
       </c>
     </row>
-    <row r="420" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A420" s="1" t="s">
         <v>7</v>
       </c>
@@ -13903,7 +13909,7 @@
         <v>123.06</v>
       </c>
     </row>
-    <row r="421" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A421" s="1" t="s">
         <v>7</v>
       </c>
@@ -13935,7 +13941,7 @@
         <v>293.97000000000003</v>
       </c>
     </row>
-    <row r="422" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A422" s="1" t="s">
         <v>7</v>
       </c>
@@ -13967,7 +13973,7 @@
         <v>590.53</v>
       </c>
     </row>
-    <row r="423" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A423" s="1" t="s">
         <v>7</v>
       </c>
@@ -13999,7 +14005,7 @@
         <v>288.19</v>
       </c>
     </row>
-    <row r="424" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A424" s="1" t="s">
         <v>7</v>
       </c>
@@ -14031,7 +14037,7 @@
         <v>354.62</v>
       </c>
     </row>
-    <row r="425" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A425" s="1" t="s">
         <v>7</v>
       </c>
@@ -14063,7 +14069,7 @@
         <v>17.84</v>
       </c>
     </row>
-    <row r="426" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A426" s="1" t="s">
         <v>7</v>
       </c>
@@ -14095,7 +14101,7 @@
         <v>186.37</v>
       </c>
     </row>
-    <row r="427" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A427" s="1" t="s">
         <v>7</v>
       </c>
@@ -14127,7 +14133,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="428" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A428" s="1" t="s">
         <v>7</v>
       </c>
@@ -14159,7 +14165,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="429" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A429" s="1" t="s">
         <v>7</v>
       </c>
@@ -14191,7 +14197,7 @@
         <v>59.94</v>
       </c>
     </row>
-    <row r="430" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A430" s="1" t="s">
         <v>7</v>
       </c>
@@ -14223,7 +14229,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="431" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A431" s="1" t="s">
         <v>7</v>
       </c>
@@ -14255,7 +14261,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="432" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A432" s="1" t="s">
         <v>7</v>
       </c>
@@ -14287,7 +14293,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="433" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A433" s="1" t="s">
         <v>7</v>
       </c>
@@ -14319,7 +14325,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="434" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A434" s="1" t="s">
         <v>7</v>
       </c>
@@ -14351,7 +14357,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="435" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A435" s="1" t="s">
         <v>7</v>
       </c>
@@ -14383,7 +14389,7 @@
         <v>405.37</v>
       </c>
     </row>
-    <row r="436" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A436" s="1" t="s">
         <v>7</v>
       </c>
@@ -14415,7 +14421,7 @@
         <v>260.14999999999998</v>
       </c>
     </row>
-    <row r="437" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A437" s="1" t="s">
         <v>7</v>
       </c>
@@ -14447,7 +14453,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="438" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A438" s="1" t="s">
         <v>7</v>
       </c>
@@ -14479,7 +14485,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="439" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A439" s="1" t="s">
         <v>7</v>
       </c>
@@ -14511,7 +14517,7 @@
         <v>150.35</v>
       </c>
     </row>
-    <row r="440" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A440" s="1" t="s">
         <v>7</v>
       </c>
@@ -14543,7 +14549,7 @@
         <v>292.47000000000003</v>
       </c>
     </row>
-    <row r="441" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A441" s="1" t="s">
         <v>7</v>
       </c>
@@ -14575,7 +14581,7 @@
         <v>105.63</v>
       </c>
     </row>
-    <row r="442" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A442" s="1" t="s">
         <v>7</v>
       </c>
@@ -14607,7 +14613,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="443" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A443" s="1" t="s">
         <v>7</v>
       </c>
@@ -14639,7 +14645,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="444" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A444" s="1" t="s">
         <v>7</v>
       </c>
@@ -14671,7 +14677,7 @@
         <v>182.31</v>
       </c>
     </row>
-    <row r="445" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A445" s="1" t="s">
         <v>7</v>
       </c>
@@ -14703,7 +14709,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="446" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A446" s="1" t="s">
         <v>7</v>
       </c>
@@ -14735,7 +14741,7 @@
         <v>125.75</v>
       </c>
     </row>
-    <row r="447" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A447" s="1" t="s">
         <v>7</v>
       </c>
@@ -14767,7 +14773,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="448" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A448" s="1" t="s">
         <v>7</v>
       </c>
@@ -14799,7 +14805,7 @@
         <v>471.45</v>
       </c>
     </row>
-    <row r="449" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A449" s="1" t="s">
         <v>7</v>
       </c>
@@ -14831,7 +14837,7 @@
         <v>397.59</v>
       </c>
     </row>
-    <row r="450" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A450" s="1" t="s">
         <v>7</v>
       </c>
@@ -14863,7 +14869,7 @@
         <v>264.57</v>
       </c>
     </row>
-    <row r="451" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A451" s="1" t="s">
         <v>7</v>
       </c>
@@ -14895,7 +14901,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="452" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A452" s="1" t="s">
         <v>7</v>
       </c>
@@ -14927,7 +14933,7 @@
         <v>360.28</v>
       </c>
     </row>
-    <row r="453" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A453" s="1" t="s">
         <v>7</v>
       </c>
@@ -14959,7 +14965,7 @@
         <v>253.31</v>
       </c>
     </row>
-    <row r="454" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A454" s="1" t="s">
         <v>7</v>
       </c>
@@ -14991,7 +14997,7 @@
         <v>239.69</v>
       </c>
     </row>
-    <row r="455" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A455" s="1" t="s">
         <v>7</v>
       </c>
@@ -15023,7 +15029,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="456" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A456" s="1" t="s">
         <v>7</v>
       </c>
@@ -15055,7 +15061,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="457" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A457" s="1" t="s">
         <v>7</v>
       </c>
@@ -15087,7 +15093,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="458" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A458" s="1" t="s">
         <v>7</v>
       </c>
@@ -15119,7 +15125,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="459" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A459" s="1" t="s">
         <v>7</v>
       </c>
@@ -15151,7 +15157,7 @@
         <v>242.61</v>
       </c>
     </row>
-    <row r="460" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="460" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A460" s="1" t="s">
         <v>7</v>
       </c>
@@ -15183,7 +15189,7 @@
         <v>56.94</v>
       </c>
     </row>
-    <row r="461" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="461" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A461" s="1" t="s">
         <v>7</v>
       </c>
@@ -15215,7 +15221,7 @@
         <v>26.25</v>
       </c>
     </row>
-    <row r="462" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="462" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A462" s="1" t="s">
         <v>7</v>
       </c>
@@ -15247,7 +15253,7 @@
         <v>391.31</v>
       </c>
     </row>
-    <row r="463" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A463" s="1" t="s">
         <v>7</v>
       </c>
@@ -15279,7 +15285,7 @@
         <v>317.47000000000003</v>
       </c>
     </row>
-    <row r="464" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="464" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A464" s="1" t="s">
         <v>7</v>
       </c>
@@ -15311,7 +15317,7 @@
         <v>445.53</v>
       </c>
     </row>
-    <row r="465" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="465" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A465" s="1" t="s">
         <v>7</v>
       </c>
@@ -15343,7 +15349,7 @@
         <v>33.840000000000003</v>
       </c>
     </row>
-    <row r="466" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="466" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A466" s="1" t="s">
         <v>7</v>
       </c>
@@ -15375,7 +15381,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="467" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="467" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A467" s="1" t="s">
         <v>7</v>
       </c>
@@ -15407,7 +15413,7 @@
         <v>432.15</v>
       </c>
     </row>
-    <row r="468" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="468" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A468" s="1" t="s">
         <v>7</v>
       </c>
@@ -15439,7 +15445,7 @@
         <v>473.47</v>
       </c>
     </row>
-    <row r="469" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="469" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A469" s="1" t="s">
         <v>7</v>
       </c>
@@ -15471,7 +15477,7 @@
         <v>147.22</v>
       </c>
     </row>
-    <row r="470" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="470" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A470" s="1" t="s">
         <v>7</v>
       </c>
@@ -15503,7 +15509,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="471" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="471" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A471" s="1" t="s">
         <v>7</v>
       </c>
@@ -15535,7 +15541,7 @@
         <v>44.07</v>
       </c>
     </row>
-    <row r="472" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="472" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A472" s="1" t="s">
         <v>7</v>
       </c>
@@ -15567,7 +15573,7 @@
         <v>500.2</v>
       </c>
     </row>
-    <row r="473" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="473" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A473" s="1" t="s">
         <v>7</v>
       </c>
@@ -15599,7 +15605,7 @@
         <v>242.78</v>
       </c>
     </row>
-    <row r="474" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="474" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A474" s="1" t="s">
         <v>7</v>
       </c>
@@ -15631,7 +15637,7 @@
         <v>315.62</v>
       </c>
     </row>
-    <row r="475" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="475" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A475" s="1" t="s">
         <v>7</v>
       </c>
@@ -15663,7 +15669,7 @@
         <v>262.64</v>
       </c>
     </row>
-    <row r="476" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="476" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A476" s="1" t="s">
         <v>7</v>
       </c>
@@ -15695,7 +15701,7 @@
         <v>64.23</v>
       </c>
     </row>
-    <row r="477" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="477" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A477" s="1" t="s">
         <v>7</v>
       </c>
@@ -15727,7 +15733,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="478" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="478" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A478" s="1" t="s">
         <v>7</v>
       </c>
@@ -15759,7 +15765,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="479" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="479" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A479" s="1" t="s">
         <v>7</v>
       </c>
@@ -15791,7 +15797,7 @@
         <v>150.81</v>
       </c>
     </row>
-    <row r="480" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="480" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A480" s="1" t="s">
         <v>8</v>
       </c>
@@ -15823,28 +15829,8 @@
         <v>600</v>
       </c>
     </row>
-    <row r="493" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A493" s="1"/>
-      <c r="B493" s="1"/>
-      <c r="C493" s="1"/>
-      <c r="D493" s="1"/>
-      <c r="E493" s="1"/>
-      <c r="F493" s="1"/>
-      <c r="G493" s="1"/>
-      <c r="H493" s="1"/>
-    </row>
-    <row r="494" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A494" s="1"/>
-      <c r="B494" s="1"/>
-      <c r="C494" s="1"/>
-      <c r="D494" s="1"/>
-      <c r="E494" s="1"/>
-      <c r="F494" s="1"/>
-      <c r="G494" s="1"/>
-      <c r="H494" s="1"/>
-    </row>
   </sheetData>
-  <sortState ref="A3:J480">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:J480">
     <sortCondition descending="1" ref="A3:A480"/>
     <sortCondition ref="C3:C480"/>
   </sortState>

</xml_diff>